<commit_message>
improved adsb mapping info
</commit_message>
<xml_diff>
--- a/doc/objects/adsb.xlsx
+++ b/doc/objects/adsb.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="496">
   <si>
     <t xml:space="preserve">COLID</t>
   </si>
@@ -1299,6 +1299,9 @@
     <t xml:space="preserve">mapping comment</t>
   </si>
   <si>
+    <t xml:space="preserve">271.L+W</t>
+  </si>
+  <si>
     <t xml:space="preserve">custom based on 150.Air Speed</t>
   </si>
   <si>
@@ -1315,6 +1318,9 @@
   </si>
   <si>
     <t xml:space="preserve">custom based on 040.ARC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not set in 100.0 in db</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -1349,7 +1355,7 @@
     <t xml:space="preserve">different</t>
   </si>
   <si>
-    <t xml:space="preserve">020.ECAT</t>
+    <t xml:space="preserve">custom based on 020.ECAT</t>
   </si>
   <si>
     <t xml:space="preserve">040.RAB</t>
@@ -1358,6 +1364,9 @@
     <t xml:space="preserve">flag</t>
   </si>
   <si>
+    <t xml:space="preserve">090.GVA</t>
+  </si>
+  <si>
     <t xml:space="preserve">157.Geometric Vertical Rate</t>
   </si>
   <si>
@@ -1382,6 +1391,9 @@
     <t xml:space="preserve">set in db but not in data?</t>
   </si>
   <si>
+    <t xml:space="preserve">TODO</t>
+  </si>
+  <si>
     <t xml:space="preserve">070.Mode-3/A</t>
   </si>
   <si>
@@ -1400,6 +1412,21 @@
     <t xml:space="preserve">090.NUCr or NACv</t>
   </si>
   <si>
+    <t xml:space="preserve">008.RA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">008.SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">008.Not TCAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flag invert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">090.PIC</t>
+  </si>
+  <si>
     <t xml:space="preserve">check if same in v8.1</t>
   </si>
   <si>
@@ -1418,12 +1445,12 @@
     <t xml:space="preserve">010.SAC</t>
   </si>
   <si>
+    <t xml:space="preserve">132.MAM</t>
+  </si>
+  <si>
     <t xml:space="preserve">040.SAA</t>
   </si>
   <si>
-    <t xml:space="preserve">flag invert</t>
-  </si>
-  <si>
     <t xml:space="preserve">015.Service Identification</t>
   </si>
   <si>
@@ -1433,12 +1460,18 @@
     <t xml:space="preserve">090.SIL</t>
   </si>
   <si>
+    <t xml:space="preserve">090.SIL-Supplement</t>
+  </si>
+  <si>
     <t xml:space="preserve">040.SIM</t>
   </si>
   <si>
     <t xml:space="preserve">200.SS</t>
   </si>
   <si>
+    <t xml:space="preserve">custom based on 200.SS</t>
+  </si>
+  <si>
     <t xml:space="preserve">080.Target Address</t>
   </si>
   <si>
@@ -1454,7 +1487,19 @@
     <t xml:space="preserve">073.Time of Message Reception for Position</t>
   </si>
   <si>
+    <t xml:space="preserve">074.FSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">074.Time of Message Reception of Position - high precision</t>
+  </si>
+  <si>
     <t xml:space="preserve">075.Time of Message Reception of Velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">076.FSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">076.Time of Message Reception of Velocity - high precision</t>
   </si>
   <si>
     <t xml:space="preserve">check mapping</t>
@@ -1476,7 +1521,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1504,11 +1549,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1559,7 +1599,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1576,7 +1616,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1584,11 +1624,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1612,10 +1648,10 @@
   <dimension ref="A1:K67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="1" sqref="E4 D33"/>
+      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.01"/>
@@ -3994,10 +4030,10 @@
   <dimension ref="A1:K96"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C70" activeCellId="1" sqref="E4 C70"/>
+      <selection pane="topLeft" activeCell="C70" activeCellId="0" sqref="C70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="64.67"/>
@@ -6152,17 +6188,17 @@
   </sheetPr>
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A85" activeCellId="0" sqref="A85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="45.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.63"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6183,6 +6219,9 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>425</v>
+      </c>
       <c r="B2" s="4"/>
       <c r="C2" s="0" t="s">
         <v>214</v>
@@ -6193,7 +6232,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>219</v>
@@ -6201,13 +6240,13 @@
       <c r="C3" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>426</v>
+      <c r="E3" s="4" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>221</v>
@@ -6215,13 +6254,13 @@
       <c r="C4" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>426</v>
+      <c r="E4" s="4" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>226</v>
@@ -6235,7 +6274,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>228</v>
@@ -6247,12 +6286,12 @@
         <v>227</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>430</v>
+      <c r="A7" s="4" t="s">
+        <v>431</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>230</v>
@@ -6263,10 +6302,13 @@
       <c r="D7" s="5" t="s">
         <v>229</v>
       </c>
+      <c r="E7" s="0" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>231</v>
@@ -6274,13 +6316,13 @@
       <c r="C8" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>432</v>
+      <c r="E8" s="6" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="0" t="s">
@@ -6301,12 +6343,12 @@
         <v>236</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>239</v>
@@ -6328,7 +6370,7 @@
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>243</v>
@@ -6340,12 +6382,12 @@
         <v>242</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>244</v>
@@ -6354,7 +6396,7 @@
         <v>244</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6365,12 +6407,12 @@
         <v>246</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C16" s="4"/>
     </row>
@@ -6384,8 +6426,8 @@
       <c r="D17" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>439</v>
+      <c r="E17" s="4" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6399,12 +6441,12 @@
         <v>250</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>441</v>
+      <c r="A19" s="4" t="s">
+        <v>443</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>253</v>
@@ -6413,7 +6455,7 @@
         <v>253</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6427,7 +6469,7 @@
         <v>254</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6441,7 +6483,7 @@
         <v>256</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6455,7 +6497,7 @@
         <v>258</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6466,7 +6508,7 @@
         <v>260</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6477,7 +6519,7 @@
         <v>261</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6488,7 +6530,7 @@
         <v>262</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6499,12 +6541,12 @@
         <v>263</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>264</v>
@@ -6512,8 +6554,8 @@
       <c r="C27" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>443</v>
+      <c r="E27" s="4" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6527,7 +6569,10 @@
         <v>266</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
+        <v>446</v>
+      </c>
       <c r="B29" s="4"/>
       <c r="C29" s="0" t="s">
         <v>270</v>
@@ -6538,7 +6583,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>271</v>
@@ -6547,12 +6592,12 @@
         <v>271</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="0" t="s">
@@ -6564,7 +6609,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>274</v>
@@ -6575,7 +6620,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>275</v>
@@ -6583,8 +6628,8 @@
       <c r="C33" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>443</v>
+      <c r="E33" s="4" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6606,7 +6651,7 @@
         <v>279</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6617,7 +6662,7 @@
         <v>280</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6631,7 +6676,7 @@
         <v>281</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6644,8 +6689,8 @@
       <c r="D38" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>439</v>
+      <c r="E38" s="4" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6655,13 +6700,13 @@
       <c r="C39" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="E39" s="6" t="s">
-        <v>437</v>
+      <c r="E39" s="4" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6" t="s">
-        <v>449</v>
+      <c r="A40" s="4" t="s">
+        <v>452</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>286</v>
@@ -6671,8 +6716,8 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6" t="s">
-        <v>449</v>
+      <c r="A41" s="4" t="s">
+        <v>452</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>287</v>
@@ -6682,8 +6727,8 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6" t="s">
-        <v>449</v>
+      <c r="A42" s="4" t="s">
+        <v>452</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>288</v>
@@ -6693,8 +6738,8 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6" t="s">
-        <v>449</v>
+      <c r="A43" s="4" t="s">
+        <v>452</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>289</v>
@@ -6705,7 +6750,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>290</v>
@@ -6713,11 +6758,14 @@
       <c r="C44" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="E44" s="6" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E44" s="4" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4" t="s">
+        <v>455</v>
+      </c>
       <c r="B45" s="4"/>
       <c r="C45" s="0" t="s">
         <v>293</v>
@@ -6725,10 +6773,13 @@
       <c r="D45" s="5" t="s">
         <v>292</v>
       </c>
+      <c r="E45" s="4" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>295</v>
@@ -6739,7 +6790,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="0" t="s">
@@ -6748,7 +6799,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="0" t="s">
@@ -6759,8 +6810,8 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>455</v>
+      <c r="A49" s="4" t="s">
+        <v>459</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="0" t="s">
@@ -6769,10 +6820,13 @@
       <c r="D49" s="5" t="s">
         <v>303</v>
       </c>
+      <c r="E49" s="4" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="0" t="s">
@@ -6784,7 +6838,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="0" t="s">
@@ -6794,7 +6848,10 @@
         <v>309</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4" t="s">
+        <v>462</v>
+      </c>
       <c r="B52" s="4"/>
       <c r="C52" s="0" t="s">
         <v>313</v>
@@ -6802,8 +6859,14 @@
       <c r="D52" s="5" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E52" s="4" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="4" t="s">
+        <v>463</v>
+      </c>
       <c r="B53" s="4"/>
       <c r="C53" s="0" t="s">
         <v>316</v>
@@ -6811,8 +6874,14 @@
       <c r="D53" s="5" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="4" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="4" t="s">
+        <v>464</v>
+      </c>
       <c r="B54" s="4"/>
       <c r="C54" s="0" t="s">
         <v>319</v>
@@ -6820,8 +6889,14 @@
       <c r="D54" s="5" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E54" s="4" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="4" t="s">
+        <v>466</v>
+      </c>
       <c r="B55" s="4"/>
       <c r="C55" s="0" t="s">
         <v>322</v>
@@ -6831,8 +6906,8 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="6" t="s">
-        <v>456</v>
+      <c r="A56" s="4" t="s">
+        <v>460</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>323</v>
@@ -6840,13 +6915,13 @@
       <c r="C56" s="0" t="s">
         <v>323</v>
       </c>
-      <c r="E56" s="6" t="s">
-        <v>458</v>
+      <c r="E56" s="4" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>459</v>
+        <v>468</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>327</v>
@@ -6858,12 +6933,12 @@
         <v>324</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>329</v>
@@ -6875,7 +6950,7 @@
         <v>328</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6940,7 +7015,7 @@
         <v>345</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6953,8 +7028,8 @@
       <c r="D65" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="E65" s="6" t="s">
-        <v>439</v>
+      <c r="E65" s="4" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6967,8 +7042,8 @@
       <c r="D66" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="E66" s="6" t="s">
-        <v>439</v>
+      <c r="E66" s="4" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6982,12 +7057,12 @@
         <v>351</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>353</v>
@@ -6998,7 +7073,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>355</v>
@@ -7010,7 +7085,10 @@
         <v>354</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="4" t="s">
+        <v>473</v>
+      </c>
       <c r="B70" s="4"/>
       <c r="C70" s="0" t="s">
         <v>358</v>
@@ -7021,7 +7099,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>464</v>
+        <v>474</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>359</v>
@@ -7029,13 +7107,13 @@
       <c r="C71" s="0" t="s">
         <v>359</v>
       </c>
-      <c r="E71" s="6" t="s">
+      <c r="E71" s="4" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>466</v>
+        <v>475</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="0" t="s">
@@ -7047,7 +7125,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>467</v>
+        <v>476</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>364</v>
@@ -7061,7 +7139,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>468</v>
+        <v>477</v>
       </c>
       <c r="B74" s="4"/>
       <c r="C74" s="0" t="s">
@@ -7071,7 +7149,10 @@
         <v>366</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="4" t="s">
+        <v>478</v>
+      </c>
       <c r="B75" s="4"/>
       <c r="C75" s="0" t="s">
         <v>370</v>
@@ -7079,10 +7160,13 @@
       <c r="D75" s="5" t="s">
         <v>369</v>
       </c>
+      <c r="E75" s="4" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>469</v>
+        <v>479</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>372</v>
@@ -7093,13 +7177,13 @@
       <c r="D76" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="E76" s="6" t="s">
-        <v>443</v>
+      <c r="E76" s="4" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>470</v>
+        <v>480</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>373</v>
@@ -7107,11 +7191,14 @@
       <c r="C77" s="0" t="s">
         <v>373</v>
       </c>
-      <c r="E77" s="6" t="s">
-        <v>443</v>
+      <c r="E77" s="4" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="4" t="s">
+        <v>481</v>
+      </c>
       <c r="B78" s="4"/>
       <c r="C78" s="0" t="s">
         <v>376</v>
@@ -7122,7 +7209,7 @@
     </row>
     <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>471</v>
+        <v>482</v>
       </c>
       <c r="B79" s="0" t="s">
         <v>378</v>
@@ -7136,7 +7223,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>472</v>
+        <v>483</v>
       </c>
       <c r="B80" s="0" t="s">
         <v>380</v>
@@ -7145,12 +7232,12 @@
         <v>380</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>473</v>
+        <v>484</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>474</v>
+        <v>485</v>
       </c>
       <c r="B81" s="0" t="s">
         <v>382</v>
@@ -7170,7 +7257,7 @@
         <v>384</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7181,12 +7268,12 @@
         <v>386</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>475</v>
+        <v>486</v>
       </c>
       <c r="B84" s="0" t="s">
         <v>390</v>
@@ -7209,7 +7296,7 @@
         <v>393</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7223,12 +7310,12 @@
         <v>395</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>475</v>
+        <v>486</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>398</v>
@@ -7237,7 +7324,10 @@
         <v>398</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="4" t="s">
+        <v>487</v>
+      </c>
       <c r="B88" s="4"/>
       <c r="C88" s="0" t="s">
         <v>401</v>
@@ -7246,7 +7336,10 @@
         <v>400</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="4" t="s">
+        <v>488</v>
+      </c>
       <c r="B89" s="4"/>
       <c r="C89" s="0" t="s">
         <v>404</v>
@@ -7257,7 +7350,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>476</v>
+        <v>489</v>
       </c>
       <c r="B90" s="0" t="s">
         <v>406</v>
@@ -7266,7 +7359,10 @@
         <v>406</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="4" t="s">
+        <v>490</v>
+      </c>
       <c r="B91" s="4"/>
       <c r="C91" s="0" t="s">
         <v>409</v>
@@ -7275,9 +7371,9 @@
         <v>408</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="6" t="s">
-        <v>476</v>
+    <row r="92" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="4" t="s">
+        <v>491</v>
       </c>
       <c r="B92" s="4"/>
       <c r="C92" s="0" t="s">
@@ -7286,13 +7382,13 @@
       <c r="D92" s="5" t="s">
         <v>411</v>
       </c>
-      <c r="E92" s="6" t="s">
-        <v>477</v>
+      <c r="E92" s="4" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>478</v>
+        <v>493</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>413</v>
@@ -7303,7 +7399,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>479</v>
+        <v>494</v>
       </c>
       <c r="B94" s="0" t="s">
         <v>414</v>
@@ -7312,12 +7408,12 @@
         <v>414</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>480</v>
+        <v>495</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>416</v>
@@ -7340,7 +7436,7 @@
         <v>417</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7351,7 +7447,7 @@
         <v>419</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>